<commit_message>
add prepare excel file
</commit_message>
<xml_diff>
--- a/app/src/data/fr_it.xlsx
+++ b/app/src/data/fr_it.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7613b76af72aef69/Documents/Programmes/Multivoc/multivoc_android/app/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ADB1EC49-1421-41E2-86B6-F3C73FCF3044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22340110-845D-46F4-95BF-891C85B39843}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{ADB1EC49-1421-41E2-86B6-F3C73FCF3044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{529497E4-B7BE-462D-96AD-AC7A59313988}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Item 1</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Item 2</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Pack</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>casa</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Bases</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>la machina, 'auto</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Objets</t>
   </si>
   <si>
@@ -106,6 +97,12 @@
   </si>
   <si>
     <t>Sat Sep 04 13:05:33 GMT+00:00 2022</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -424,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,39 +441,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -490,19 +487,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -516,19 +513,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -542,19 +539,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
@@ -568,19 +565,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -590,6 +587,14 @@
       </c>
       <c r="H6" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>